<commit_message>
Aiged and Canton decks
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snidersa\git\CKCG-card-maker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansarij\Winter-22-Workspace\CrimsonKnights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C071562-C8D2-4373-A1C4-6D4F1A796251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA80C5-BB16-4489-BBDA-C705DF15E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -45,28 +45,250 @@
     <t>C</t>
   </si>
   <si>
-    <t>Test creature</t>
-  </si>
-  <si>
-    <t>Test Spell</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
-    <t>Test Spell Description</t>
-  </si>
-  <si>
-    <t>Test Creature description</t>
-  </si>
-  <si>
     <t>Character</t>
   </si>
   <si>
-    <t>Character 1</t>
-  </si>
-  <si>
-    <t>Character 2</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Canton</t>
+  </si>
+  <si>
+    <t>Wand of the War Mage</t>
+  </si>
+  <si>
+    <t>Pearl of Power</t>
+  </si>
+  <si>
+    <t>Irradianus Mundi</t>
+  </si>
+  <si>
+    <t>Once 8 spells have been in your discard pile, equip this. As an action, you can play a spell from your discard pile as long as there is 2 copies of it in the discard pile and isn't a reaction.</t>
+  </si>
+  <si>
+    <t>After you have played 4 spells from hand this game, equip this. Once per game, you can roll 1d4 and add up to that many spells from your discard pile to your hand. Those choosen spells don't count against you max hand size until used.</t>
+  </si>
+  <si>
+    <t>When you have shuffled 3 spells back into your deck, equip this. Your hero's passive does 2 additional damage.</t>
+  </si>
+  <si>
+    <t>Canicus</t>
+  </si>
+  <si>
+    <t>The first time you cast a spell in a turn, you can play a spell from your discard pile.</t>
+  </si>
+  <si>
+    <t>Bend Luck</t>
+  </si>
+  <si>
+    <t>Choose a player and send one of their cards either on the field, hand, or top card of their deck to the discard pile.</t>
+  </si>
+  <si>
+    <t>Corrosive Cage</t>
+  </si>
+  <si>
+    <t>When drawn, place this card on the field. It is dormant and can't be effected. Whenever a "Crafting Component" card is played, attach to this card.  When this card gets 2 "Crafting Components", it becomes no longer dormant and equips to the hero. While not dormant, you can use a reaction to trap a card being played inside. While trapped the card cannot be played, and it takes an action for the cards owner to add it back to their hand. Only one card can be held at a time.</t>
+  </si>
+  <si>
+    <t>Crafting Component</t>
+  </si>
+  <si>
+    <t>Finding Evidence</t>
+  </si>
+  <si>
+    <t>Choose an enemy hero, equip this to them. Each instance of damage you deal with spells against that target will deal 1 more damage. When that hero dies, you heal 10 HP.</t>
+  </si>
+  <si>
+    <t>Preparing Ingredients</t>
+  </si>
+  <si>
+    <t>Take 2 cards of your choice out of the deck, shuffle your deck, and then place those 2 cards on top of the deck in any order. Draw 2 cards on your next turn.</t>
+  </si>
+  <si>
+    <t>Presenting a Case</t>
+  </si>
+  <si>
+    <t>If this is not drawn by "Finding Evidence", shuffle this card back into the deck and draw again. Play all 3 cards that are out of the game and then shuffle this card and "Finding Evidence" back into the deck.</t>
+  </si>
+  <si>
+    <t>Raven Queen's Fate</t>
+  </si>
+  <si>
+    <t>Take 3 cards of your choice out of the deck and place them in your hand, then shuffle the deck. These 3 cards don't count against you max hand size and you must discard 3 cards at the end of your next turn.</t>
+  </si>
+  <si>
+    <t>Sorcery Points</t>
+  </si>
+  <si>
+    <t>Add a card from your discard pile to your hand, then play another card.</t>
+  </si>
+  <si>
+    <t>Tides of Chaos</t>
+  </si>
+  <si>
+    <t>When your opponent plays a card, pick a card randomly from their hand to play instead. If "Wild Magic Surge" is in the discard pile, add it to your hand.</t>
+  </si>
+  <si>
+    <t>Wild Magic Surge</t>
+  </si>
+  <si>
+    <t>Roll a d20,  on a 1 discard your hand, on a 2 to 10 you can play a spell from your discard pile and then add it to your hand, on a 11 to 19 you draw a card and then play a spell card from your hand, on a 20 you roll 2 more times (rerolling any 1s or repeat 20s.)</t>
+  </si>
+  <si>
+    <t>Agonizing Blast</t>
+  </si>
+  <si>
+    <t>Dimension Door</t>
+  </si>
+  <si>
+    <t>Counterspell</t>
+  </si>
+  <si>
+    <t>Repelling Blast</t>
+  </si>
+  <si>
+    <t>Telekinesis</t>
+  </si>
+  <si>
+    <t>Vortex Warp</t>
+  </si>
+  <si>
+    <t>1d4+2</t>
+  </si>
+  <si>
+    <t>Deal 1d4+2 damage to a enemy of your choice.</t>
+  </si>
+  <si>
+    <t>Draw a card and then remove the top card from an opponents deck of your choice.</t>
+  </si>
+  <si>
+    <t>Take a another card in you hand and switch it out with a card of your choice in your deck, then shuffle your deck.</t>
+  </si>
+  <si>
+    <t>Select an enemy, Deal 2 damage to it and have its current player send a random card from their hand back to the top of their deck.</t>
+  </si>
+  <si>
+    <t>Take up to two cards from your deck or discard pile and add it to your hand, then look in your opponents hand and shuffle one of those cards into that player's deck.</t>
+  </si>
+  <si>
+    <t>Take a card on the field or hand and shuffle it into its owner's deck, or add a card from your discard pile to your hand.</t>
+  </si>
+  <si>
+    <t>Hexblade's Curse</t>
+  </si>
+  <si>
+    <t>Equip to your hero. The first time you would play a non-comapnion card on a turn, set it outside the game instead of in the discard pile. Once you have 3 cards set aside, draw "Presenting Case"</t>
+  </si>
+  <si>
+    <t>If you draw this card while not having a "Craftable" card on the field, shuffle this back into your deck a draw again. If there is a "Craftable" card in the field, play it immediately and your hero gains +1 AC permanently.</t>
+  </si>
+  <si>
+    <t>Claw</t>
+  </si>
+  <si>
+    <t>Aiged</t>
+  </si>
+  <si>
+    <t>+3 attack, When you attack an opponent's hero, you can add a card from your discard pile to your hand except "Taxes" and it cannot be played that turn.</t>
+  </si>
+  <si>
+    <t>Seaweave Boat</t>
+  </si>
+  <si>
+    <t>+2 AC, As an action you can select an opponent, then you both randomly choose a card in each others hand to discard.</t>
+  </si>
+  <si>
+    <t>Wilhelm</t>
+  </si>
+  <si>
+    <t>When this card is played, equip a tax gold from a players deck to this card. When this dies, attach the tax gold to Aiged.</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Choose an opponent and search their deck, if you find a "Tax Gold" card, attach it to Aiged.</t>
+  </si>
+  <si>
+    <t>Tax Gold</t>
+  </si>
+  <si>
+    <t>Draw 2 cards. When played or discarded, attach it to Aiged.</t>
+  </si>
+  <si>
+    <t>Battle Miniatures</t>
+  </si>
+  <si>
+    <t>Opponents cannot target you with cards and attacks while you have this minion on your field.</t>
+  </si>
+  <si>
+    <t>Fire Breath</t>
+  </si>
+  <si>
+    <t>Planetar Form</t>
+  </si>
+  <si>
+    <t>Equip this to your hero until the end of your second turn. While equipped, you hero doesn't take damage when attacking and can use an action to heal 1d8.</t>
+  </si>
+  <si>
+    <t>This is a public Spa!</t>
+  </si>
+  <si>
+    <t>All minions on the field are returned to their owner's hands. If there are none draw, 2 cards instead.</t>
+  </si>
+  <si>
+    <t>Radiant Breath</t>
+  </si>
+  <si>
+    <t>Select an opponent, that opponent and their minions take 2 damage and cannot attack until the end of your next turn</t>
+  </si>
+  <si>
+    <t>Select two cards in an opponents hand of your choice and discard them, any "Tax Gold" cards are attached to Aiged.</t>
+  </si>
+  <si>
+    <t>Choose up to 5 minions or opponents of your choice and deal 2 damage to each of them, ignoring AC.</t>
+  </si>
+  <si>
+    <t>Gold Eater</t>
+  </si>
+  <si>
+    <t>Human Form</t>
+  </si>
+  <si>
+    <t>Heal 1d4 and equip this to your hero until the end of your second turn. While equipped, when you draw a card during your draw phase you may place it at the bottom of your deck and draw another, once.</t>
+  </si>
+  <si>
+    <t>Divine Awareness</t>
+  </si>
+  <si>
+    <t>Select an opponent and look at their hand. If they are holding a "Tax Gold" card, they must discard one card of their choice.</t>
+  </si>
+  <si>
+    <t>Come Pick Us Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select an opponent then you and that opponent shuffle your hands into your decks, then draw cards equal to the amount shuffled + 1. </t>
+  </si>
+  <si>
+    <t>Tactical Minitures</t>
+  </si>
+  <si>
+    <t>Heretical Divide</t>
+  </si>
+  <si>
+    <t>If this minion is alive during your next beginning phase, destroy it and draw a card.</t>
+  </si>
+  <si>
+    <t>Until the end of your next turn, any time an opponent would either use an action or attack with a minion or hero, they must send the top card of their deck to the discard pile. Any "Tax Gold" sent it attached to Aiged instead.</t>
   </si>
 </sst>
 </file>
@@ -384,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -409,32 +631,32 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -443,13 +665,713 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>34</v>
+      </c>
+      <c r="F30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed decimals on AC and added instructions
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\snidersa\git\CrimsonKnights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D847FC6-4DD1-42F8-BC73-B43D8DA26F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1736FBA7-D88B-46C7-A63A-6B27ED2C3D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,9 +285,6 @@
     <t>While attacking, you take no damage in return.</t>
   </si>
   <si>
-    <t>Tyrael</t>
-  </si>
-  <si>
     <t>Gauntlet</t>
   </si>
   <si>
@@ -1309,6 +1306,9 @@
   </si>
   <si>
     <t>(Craftable) When drawn, place this card on the field. It is dormant and can't be effected. Whenever a "Crafting Component" card is played, attach to this card. When this card gets 2 "Crafting Components", it becomes no longer dormant and equips to the hero. While not dormant, you can use a reaction to trap a card being played inside. While trapped the card cannot be played, and it takes an action for the cards owner to add it back to their hand. Only one card can be held at a time.</t>
+  </si>
+  <si>
+    <t>Tyreal</t>
   </si>
 </sst>
 </file>
@@ -1344,9 +1344,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1629,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="H180" sqref="H180"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1672,12 +1673,12 @@
         <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1686,32 +1687,32 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F4" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -1720,15 +1721,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -1737,15 +1738,15 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -1757,15 +1758,15 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
         <v>5</v>
@@ -1777,15 +1778,15 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -1797,239 +1798,239 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
         <v>100</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>103</v>
-      </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
         <v>104</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>105</v>
-      </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
         <v>106</v>
       </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>107</v>
-      </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
         <v>108</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>109</v>
-      </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
         <v>110</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>111</v>
-      </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
         <v>114</v>
       </c>
-      <c r="B17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>115</v>
-      </c>
       <c r="F17" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
         <v>116</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>117</v>
-      </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
         <v>118</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>119</v>
-      </c>
       <c r="F19" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
         <v>120</v>
       </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" t="s">
-        <v>121</v>
-      </c>
       <c r="F20" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
         <v>122</v>
       </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" t="s">
-        <v>123</v>
-      </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
         <v>124</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>125</v>
-      </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
         <v>128</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>129</v>
-      </c>
       <c r="F24" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
         <v>130</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>131</v>
-      </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -2038,15 +2039,15 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" t="s">
         <v>133</v>
-      </c>
-      <c r="F26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
@@ -2055,15 +2056,15 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
@@ -2075,12 +2076,12 @@
         <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -2092,15 +2093,15 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
@@ -2112,15 +2113,15 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B31" t="s">
         <v>5</v>
@@ -2132,15 +2133,15 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
@@ -2152,10 +2153,10 @@
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2169,194 +2170,194 @@
         <v>33</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
         <v>146</v>
       </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>147</v>
-      </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
         <v>148</v>
       </c>
-      <c r="B35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>149</v>
-      </c>
       <c r="F35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B36" t="s">
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>151</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
         <v>152</v>
       </c>
-      <c r="B37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>153</v>
-      </c>
       <c r="F37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
         <v>154</v>
       </c>
-      <c r="B38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>155</v>
-      </c>
       <c r="F38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B39" t="s">
         <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
         <v>160</v>
       </c>
-      <c r="B41" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" t="s">
-        <v>161</v>
-      </c>
       <c r="F41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>161</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
         <v>162</v>
       </c>
-      <c r="B42" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>163</v>
-      </c>
       <c r="F42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
         <v>164</v>
       </c>
-      <c r="B43" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>165</v>
-      </c>
       <c r="F43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
         <v>166</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
-      </c>
-      <c r="E44" t="s">
-        <v>167</v>
-      </c>
       <c r="F44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
         <v>168</v>
       </c>
-      <c r="B45" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" t="s">
-        <v>169</v>
-      </c>
       <c r="F45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
         <v>170</v>
       </c>
-      <c r="B46" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" t="s">
-        <v>171</v>
-      </c>
       <c r="F46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
@@ -2368,15 +2369,15 @@
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -2385,15 +2386,15 @@
         <v>1</v>
       </c>
       <c r="E48" t="s">
+        <v>174</v>
+      </c>
+      <c r="F48" t="s">
         <v>175</v>
-      </c>
-      <c r="F48" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -2402,15 +2403,15 @@
         <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B50" t="s">
         <v>8</v>
@@ -2419,15 +2420,15 @@
         <v>2</v>
       </c>
       <c r="E50" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F50" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -2439,15 +2440,15 @@
         <v>3</v>
       </c>
       <c r="E51" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F51" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
@@ -2459,15 +2460,15 @@
         <v>3</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F52" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -2479,71 +2480,71 @@
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B54" t="s">
         <v>10</v>
       </c>
       <c r="E54" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>188</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
         <v>189</v>
       </c>
-      <c r="B55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" t="s">
-        <v>190</v>
-      </c>
       <c r="F55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
         <v>191</v>
       </c>
-      <c r="B56" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" t="s">
-        <v>192</v>
-      </c>
       <c r="F56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>192</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
         <v>193</v>
       </c>
-      <c r="B57" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" t="s">
-        <v>194</v>
-      </c>
       <c r="F57" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -2552,147 +2553,147 @@
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
         <v>196</v>
       </c>
-      <c r="B59" t="s">
-        <v>6</v>
-      </c>
-      <c r="E59" t="s">
-        <v>197</v>
-      </c>
       <c r="F59" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
         <v>198</v>
       </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" t="s">
-        <v>199</v>
-      </c>
       <c r="F60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
         <v>200</v>
       </c>
-      <c r="B61" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" t="s">
-        <v>201</v>
-      </c>
       <c r="F61" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
         <v>202</v>
       </c>
-      <c r="B62" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" t="s">
-        <v>203</v>
-      </c>
       <c r="F62" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>203</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
         <v>204</v>
       </c>
-      <c r="B63" t="s">
-        <v>6</v>
-      </c>
-      <c r="E63" t="s">
-        <v>205</v>
-      </c>
       <c r="F63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
         <v>206</v>
       </c>
-      <c r="B64" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" t="s">
-        <v>207</v>
-      </c>
       <c r="F64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
         <v>208</v>
       </c>
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-      <c r="E65" t="s">
-        <v>209</v>
-      </c>
       <c r="F65" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
         <v>210</v>
       </c>
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" t="s">
-        <v>211</v>
-      </c>
       <c r="F66" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>211</v>
+      </c>
+      <c r="B67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
         <v>212</v>
       </c>
-      <c r="B67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" t="s">
-        <v>213</v>
-      </c>
       <c r="F67" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>213</v>
+      </c>
+      <c r="B68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
         <v>214</v>
       </c>
-      <c r="B68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" t="s">
-        <v>215</v>
-      </c>
       <c r="F68" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2817,7 +2818,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -2969,7 +2970,7 @@
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F82" t="s">
         <v>54</v>
@@ -3129,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="E90" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F90" t="s">
         <v>11</v>
@@ -3309,7 +3310,7 @@
         <v>0</v>
       </c>
       <c r="E99" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F99" t="s">
         <v>11</v>
@@ -3437,7 +3438,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
@@ -3449,15 +3450,15 @@
         <v>0</v>
       </c>
       <c r="E106" t="s">
+        <v>218</v>
+      </c>
+      <c r="F106" t="s">
         <v>219</v>
-      </c>
-      <c r="F106" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
@@ -3469,15 +3470,15 @@
         <v>0</v>
       </c>
       <c r="E107" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B108" t="s">
         <v>8</v>
@@ -3489,167 +3490,167 @@
         <v>1</v>
       </c>
       <c r="E108" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F108" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>224</v>
+      </c>
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
         <v>225</v>
       </c>
-      <c r="B109" t="s">
-        <v>6</v>
-      </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109" t="s">
-        <v>226</v>
-      </c>
       <c r="F109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>226</v>
+      </c>
+      <c r="B110" t="s">
+        <v>6</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
         <v>227</v>
       </c>
-      <c r="B110" t="s">
-        <v>6</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-      <c r="E110" t="s">
-        <v>228</v>
-      </c>
       <c r="F110" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
       </c>
       <c r="E111" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F111" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>230</v>
+      </c>
+      <c r="B112" t="s">
+        <v>6</v>
+      </c>
+      <c r="E112" t="s">
         <v>231</v>
       </c>
-      <c r="B112" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" t="s">
-        <v>232</v>
-      </c>
       <c r="F112" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="E113" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>233</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+      <c r="E114" t="s">
         <v>234</v>
       </c>
-      <c r="B114" t="s">
-        <v>6</v>
-      </c>
-      <c r="E114" t="s">
-        <v>235</v>
-      </c>
       <c r="F114" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B115" t="s">
         <v>10</v>
       </c>
       <c r="E115" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F115" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>237</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="E116" t="s">
         <v>238</v>
       </c>
-      <c r="B116" t="s">
-        <v>6</v>
-      </c>
-      <c r="E116" t="s">
-        <v>239</v>
-      </c>
       <c r="F116" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
+        <v>239</v>
+      </c>
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E117" t="s">
         <v>240</v>
       </c>
-      <c r="B117" t="s">
-        <v>6</v>
-      </c>
-      <c r="E117" t="s">
-        <v>241</v>
-      </c>
       <c r="F117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>241</v>
+      </c>
+      <c r="B118" t="s">
+        <v>6</v>
+      </c>
+      <c r="E118" t="s">
         <v>242</v>
       </c>
-      <c r="B118" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" t="s">
-        <v>243</v>
-      </c>
       <c r="F118" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
@@ -3661,15 +3662,15 @@
         <v>8</v>
       </c>
       <c r="E119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
@@ -3681,15 +3682,15 @@
         <v>2</v>
       </c>
       <c r="E120" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F120" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B121" t="s">
         <v>5</v>
@@ -3701,15 +3702,15 @@
         <v>3</v>
       </c>
       <c r="E121" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F121" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
@@ -3721,113 +3722,113 @@
         <v>5</v>
       </c>
       <c r="E122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F122" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>251</v>
+      </c>
+      <c r="B123" t="s">
+        <v>6</v>
+      </c>
+      <c r="E123" t="s">
         <v>252</v>
       </c>
-      <c r="B123" t="s">
-        <v>6</v>
-      </c>
-      <c r="E123" t="s">
-        <v>253</v>
-      </c>
       <c r="F123" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>253</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="E124" t="s">
         <v>254</v>
       </c>
-      <c r="B124" t="s">
-        <v>6</v>
-      </c>
-      <c r="E124" t="s">
-        <v>255</v>
-      </c>
       <c r="F124" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>255</v>
+      </c>
+      <c r="B125" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" t="s">
         <v>256</v>
       </c>
-      <c r="B125" t="s">
-        <v>6</v>
-      </c>
-      <c r="E125" t="s">
-        <v>257</v>
-      </c>
       <c r="F125" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>257</v>
+      </c>
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" t="s">
         <v>258</v>
       </c>
-      <c r="B126" t="s">
-        <v>6</v>
-      </c>
-      <c r="E126" t="s">
-        <v>259</v>
-      </c>
       <c r="F126" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>259</v>
+      </c>
+      <c r="B127" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" t="s">
         <v>260</v>
       </c>
-      <c r="B127" t="s">
-        <v>6</v>
-      </c>
-      <c r="E127" t="s">
-        <v>261</v>
-      </c>
       <c r="F127" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
+        <v>261</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="E128" t="s">
         <v>262</v>
       </c>
-      <c r="B128" t="s">
-        <v>6</v>
-      </c>
-      <c r="E128" t="s">
-        <v>263</v>
-      </c>
       <c r="F128" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
+        <v>263</v>
+      </c>
+      <c r="B129" t="s">
+        <v>6</v>
+      </c>
+      <c r="E129" t="s">
         <v>264</v>
       </c>
-      <c r="B129" t="s">
-        <v>6</v>
-      </c>
-      <c r="E129" t="s">
-        <v>265</v>
-      </c>
       <c r="F129" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B130" t="s">
         <v>9</v>
@@ -3839,15 +3840,15 @@
         <v>0</v>
       </c>
       <c r="E130" t="s">
+        <v>266</v>
+      </c>
+      <c r="F130" t="s">
         <v>267</v>
-      </c>
-      <c r="F130" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B131" t="s">
         <v>8</v>
@@ -3859,15 +3860,15 @@
         <v>2</v>
       </c>
       <c r="E131" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F131" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B132" t="s">
         <v>8</v>
@@ -3879,15 +3880,15 @@
         <v>0</v>
       </c>
       <c r="E132" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F132" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
@@ -3899,15 +3900,15 @@
         <v>6</v>
       </c>
       <c r="E133" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F133" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
@@ -3919,15 +3920,15 @@
         <v>4</v>
       </c>
       <c r="E134" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F134" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
@@ -3939,239 +3940,239 @@
         <v>3</v>
       </c>
       <c r="E135" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F135" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
+        <v>278</v>
+      </c>
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="E136" t="s">
         <v>279</v>
       </c>
-      <c r="B136" t="s">
-        <v>6</v>
-      </c>
-      <c r="E136" t="s">
-        <v>280</v>
-      </c>
       <c r="F136" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>280</v>
+      </c>
+      <c r="B137" t="s">
+        <v>6</v>
+      </c>
+      <c r="E137" t="s">
         <v>281</v>
       </c>
-      <c r="B137" t="s">
-        <v>6</v>
-      </c>
-      <c r="E137" t="s">
-        <v>282</v>
-      </c>
       <c r="F137" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>282</v>
+      </c>
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="E138" t="s">
         <v>283</v>
       </c>
-      <c r="B138" t="s">
-        <v>6</v>
-      </c>
-      <c r="E138" t="s">
-        <v>284</v>
-      </c>
       <c r="F138" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>284</v>
+      </c>
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="E139" t="s">
         <v>285</v>
       </c>
-      <c r="B139" t="s">
-        <v>6</v>
-      </c>
-      <c r="E139" t="s">
-        <v>286</v>
-      </c>
       <c r="F139" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
+        <v>286</v>
+      </c>
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="E140" t="s">
         <v>287</v>
       </c>
-      <c r="B140" t="s">
-        <v>6</v>
-      </c>
-      <c r="E140" t="s">
-        <v>288</v>
-      </c>
       <c r="F140" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
+        <v>288</v>
+      </c>
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="E141" t="s">
         <v>289</v>
       </c>
-      <c r="B141" t="s">
-        <v>6</v>
-      </c>
-      <c r="E141" t="s">
-        <v>290</v>
-      </c>
       <c r="F141" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
+        <v>290</v>
+      </c>
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="E142" t="s">
         <v>291</v>
       </c>
-      <c r="B142" t="s">
-        <v>6</v>
-      </c>
-      <c r="E142" t="s">
-        <v>292</v>
-      </c>
       <c r="F142" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
+        <v>292</v>
+      </c>
+      <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="E143" t="s">
         <v>293</v>
       </c>
-      <c r="B143" t="s">
-        <v>6</v>
-      </c>
-      <c r="E143" t="s">
-        <v>294</v>
-      </c>
       <c r="F143" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
+        <v>294</v>
+      </c>
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="E144" t="s">
         <v>295</v>
       </c>
-      <c r="B144" t="s">
-        <v>6</v>
-      </c>
-      <c r="E144" t="s">
-        <v>296</v>
-      </c>
       <c r="F144" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
+        <v>296</v>
+      </c>
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+      <c r="E145" t="s">
         <v>297</v>
       </c>
-      <c r="B145" t="s">
-        <v>6</v>
-      </c>
-      <c r="E145" t="s">
-        <v>298</v>
-      </c>
       <c r="F145" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
+        <v>298</v>
+      </c>
+      <c r="B146" t="s">
+        <v>6</v>
+      </c>
+      <c r="E146" t="s">
         <v>299</v>
       </c>
-      <c r="B146" t="s">
-        <v>6</v>
-      </c>
-      <c r="E146" t="s">
-        <v>300</v>
-      </c>
       <c r="F146" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
+        <v>300</v>
+      </c>
+      <c r="B147" t="s">
+        <v>6</v>
+      </c>
+      <c r="E147" t="s">
         <v>301</v>
       </c>
-      <c r="B147" t="s">
-        <v>6</v>
-      </c>
-      <c r="E147" t="s">
-        <v>302</v>
-      </c>
       <c r="F147" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
+        <v>302</v>
+      </c>
+      <c r="B148" t="s">
+        <v>6</v>
+      </c>
+      <c r="E148" t="s">
         <v>303</v>
       </c>
-      <c r="B148" t="s">
-        <v>6</v>
-      </c>
-      <c r="E148" t="s">
-        <v>304</v>
-      </c>
       <c r="F148" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
+        <v>304</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="E149" t="s">
         <v>305</v>
       </c>
-      <c r="B149" t="s">
-        <v>6</v>
-      </c>
-      <c r="E149" t="s">
-        <v>306</v>
-      </c>
       <c r="F149" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B150" t="s">
         <v>10</v>
       </c>
       <c r="E150" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F150" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B151" t="s">
         <v>10</v>
       </c>
       <c r="E151" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F151" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B152" t="s">
         <v>9</v>
@@ -4183,15 +4184,15 @@
         <v>0</v>
       </c>
       <c r="E152" t="s">
+        <v>311</v>
+      </c>
+      <c r="F152" t="s">
         <v>312</v>
-      </c>
-      <c r="F152" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B153" t="s">
         <v>8</v>
@@ -4203,15 +4204,15 @@
         <v>0</v>
       </c>
       <c r="E153" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F153" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B154" t="s">
         <v>5</v>
@@ -4223,12 +4224,12 @@
         <v>1</v>
       </c>
       <c r="F154" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B155" t="s">
         <v>5</v>
@@ -4240,15 +4241,15 @@
         <v>3</v>
       </c>
       <c r="E155" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F155" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B156" t="s">
         <v>5</v>
@@ -4260,15 +4261,15 @@
         <v>2</v>
       </c>
       <c r="E156" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F156" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B157" t="s">
         <v>5</v>
@@ -4280,15 +4281,15 @@
         <v>1</v>
       </c>
       <c r="E157" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F157" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B158" t="s">
         <v>5</v>
@@ -4300,211 +4301,211 @@
         <v>4</v>
       </c>
       <c r="E158" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F158" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
+        <v>324</v>
+      </c>
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+      <c r="E159" t="s">
         <v>325</v>
       </c>
-      <c r="B159" t="s">
-        <v>6</v>
-      </c>
-      <c r="E159" t="s">
-        <v>326</v>
-      </c>
       <c r="F159" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
+        <v>326</v>
+      </c>
+      <c r="B160" t="s">
+        <v>6</v>
+      </c>
+      <c r="E160" t="s">
         <v>327</v>
       </c>
-      <c r="B160" t="s">
-        <v>6</v>
-      </c>
-      <c r="E160" t="s">
-        <v>328</v>
-      </c>
       <c r="F160" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B161" t="s">
         <v>10</v>
       </c>
       <c r="E161" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F161" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
+        <v>330</v>
+      </c>
+      <c r="B162" t="s">
+        <v>6</v>
+      </c>
+      <c r="E162" t="s">
         <v>331</v>
       </c>
-      <c r="B162" t="s">
-        <v>6</v>
-      </c>
-      <c r="E162" t="s">
-        <v>332</v>
-      </c>
       <c r="F162" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
+        <v>332</v>
+      </c>
+      <c r="B163" t="s">
+        <v>6</v>
+      </c>
+      <c r="E163" t="s">
         <v>333</v>
       </c>
-      <c r="B163" t="s">
-        <v>6</v>
-      </c>
-      <c r="E163" t="s">
-        <v>334</v>
-      </c>
       <c r="F163" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
+        <v>334</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="E164" t="s">
         <v>335</v>
       </c>
-      <c r="B164" t="s">
-        <v>6</v>
-      </c>
-      <c r="E164" t="s">
-        <v>336</v>
-      </c>
       <c r="F164" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
+        <v>336</v>
+      </c>
+      <c r="B165" t="s">
+        <v>6</v>
+      </c>
+      <c r="E165" t="s">
         <v>337</v>
       </c>
-      <c r="B165" t="s">
-        <v>6</v>
-      </c>
-      <c r="E165" t="s">
-        <v>338</v>
-      </c>
       <c r="F165" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
+        <v>338</v>
+      </c>
+      <c r="B166" t="s">
+        <v>6</v>
+      </c>
+      <c r="E166" t="s">
         <v>339</v>
       </c>
-      <c r="B166" t="s">
-        <v>6</v>
-      </c>
-      <c r="E166" t="s">
-        <v>340</v>
-      </c>
       <c r="F166" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
+        <v>340</v>
+      </c>
+      <c r="B167" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" t="s">
         <v>341</v>
       </c>
-      <c r="B167" t="s">
-        <v>6</v>
-      </c>
-      <c r="E167" t="s">
-        <v>342</v>
-      </c>
       <c r="F167" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
+        <v>342</v>
+      </c>
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" t="s">
         <v>343</v>
       </c>
-      <c r="B168" t="s">
-        <v>6</v>
-      </c>
-      <c r="E168" t="s">
-        <v>344</v>
-      </c>
       <c r="F168" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
+        <v>344</v>
+      </c>
+      <c r="B169" t="s">
+        <v>6</v>
+      </c>
+      <c r="E169" t="s">
         <v>345</v>
       </c>
-      <c r="B169" t="s">
-        <v>6</v>
-      </c>
-      <c r="E169" t="s">
-        <v>346</v>
-      </c>
       <c r="F169" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" t="s">
+        <v>6</v>
+      </c>
+      <c r="E170" t="s">
         <v>347</v>
       </c>
-      <c r="B170" t="s">
-        <v>6</v>
-      </c>
-      <c r="E170" t="s">
-        <v>348</v>
-      </c>
       <c r="F170" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B171" t="s">
         <v>10</v>
       </c>
       <c r="E171" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F171" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B172" t="s">
         <v>10</v>
       </c>
       <c r="E172" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F172" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B173" t="s">
         <v>9</v>
@@ -4516,15 +4517,15 @@
         <v>0</v>
       </c>
       <c r="E173" t="s">
+        <v>353</v>
+      </c>
+      <c r="F173" t="s">
         <v>354</v>
-      </c>
-      <c r="F173" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B174" t="s">
         <v>8</v>
@@ -4536,29 +4537,29 @@
         <v>3</v>
       </c>
       <c r="E174" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F174" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B175" t="s">
         <v>8</v>
       </c>
       <c r="E175" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F175" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B176" t="s">
         <v>5</v>
@@ -4570,253 +4571,253 @@
         <v>5</v>
       </c>
       <c r="E176" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F176" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
+        <v>361</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="E177" t="s">
         <v>362</v>
       </c>
-      <c r="B177" t="s">
-        <v>6</v>
-      </c>
-      <c r="E177" t="s">
-        <v>363</v>
-      </c>
       <c r="F177" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
+        <v>363</v>
+      </c>
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="E178" t="s">
         <v>364</v>
       </c>
-      <c r="B178" t="s">
-        <v>6</v>
-      </c>
-      <c r="E178" t="s">
-        <v>365</v>
-      </c>
       <c r="F178" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
+        <v>365</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="E179" t="s">
         <v>366</v>
       </c>
-      <c r="B179" t="s">
-        <v>6</v>
-      </c>
-      <c r="E179" t="s">
-        <v>367</v>
-      </c>
       <c r="F179" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
+        <v>367</v>
+      </c>
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="E180" t="s">
         <v>368</v>
       </c>
-      <c r="B180" t="s">
-        <v>6</v>
-      </c>
-      <c r="E180" t="s">
-        <v>369</v>
-      </c>
       <c r="F180" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
+        <v>369</v>
+      </c>
+      <c r="B181" t="s">
+        <v>6</v>
+      </c>
+      <c r="E181" t="s">
         <v>370</v>
       </c>
-      <c r="B181" t="s">
-        <v>6</v>
-      </c>
-      <c r="E181" t="s">
-        <v>371</v>
-      </c>
       <c r="F181" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
       </c>
       <c r="E182" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F182" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
+        <v>230</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="E183" t="s">
         <v>231</v>
       </c>
-      <c r="B183" t="s">
-        <v>6</v>
-      </c>
-      <c r="E183" t="s">
-        <v>232</v>
-      </c>
       <c r="F183" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
+        <v>224</v>
+      </c>
+      <c r="B184" t="s">
+        <v>6</v>
+      </c>
+      <c r="E184" t="s">
         <v>225</v>
       </c>
-      <c r="B184" t="s">
-        <v>6</v>
-      </c>
-      <c r="E184" t="s">
-        <v>226</v>
-      </c>
       <c r="F184" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
+        <v>372</v>
+      </c>
+      <c r="B185" t="s">
+        <v>6</v>
+      </c>
+      <c r="E185" t="s">
         <v>373</v>
       </c>
-      <c r="B185" t="s">
-        <v>6</v>
-      </c>
-      <c r="E185" t="s">
-        <v>374</v>
-      </c>
       <c r="F185" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
+        <v>374</v>
+      </c>
+      <c r="B186" t="s">
+        <v>6</v>
+      </c>
+      <c r="E186" t="s">
         <v>375</v>
       </c>
-      <c r="B186" t="s">
-        <v>6</v>
-      </c>
-      <c r="E186" t="s">
-        <v>376</v>
-      </c>
       <c r="F186" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
+        <v>376</v>
+      </c>
+      <c r="B187" t="s">
+        <v>6</v>
+      </c>
+      <c r="E187" t="s">
         <v>377</v>
       </c>
-      <c r="B187" t="s">
-        <v>6</v>
-      </c>
-      <c r="E187" t="s">
-        <v>378</v>
-      </c>
       <c r="F187" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
+        <v>378</v>
+      </c>
+      <c r="B188" t="s">
+        <v>6</v>
+      </c>
+      <c r="E188" t="s">
         <v>379</v>
       </c>
-      <c r="B188" t="s">
-        <v>6</v>
-      </c>
-      <c r="E188" t="s">
-        <v>380</v>
-      </c>
       <c r="F188" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
+        <v>380</v>
+      </c>
+      <c r="B189" t="s">
+        <v>6</v>
+      </c>
+      <c r="E189" t="s">
         <v>381</v>
       </c>
-      <c r="B189" t="s">
-        <v>6</v>
-      </c>
-      <c r="E189" t="s">
-        <v>382</v>
-      </c>
       <c r="F189" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
+        <v>382</v>
+      </c>
+      <c r="B190" t="s">
+        <v>6</v>
+      </c>
+      <c r="E190" t="s">
         <v>383</v>
       </c>
-      <c r="B190" t="s">
-        <v>6</v>
-      </c>
-      <c r="E190" t="s">
-        <v>384</v>
-      </c>
       <c r="F190" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
+        <v>384</v>
+      </c>
+      <c r="B191" t="s">
+        <v>6</v>
+      </c>
+      <c r="E191" t="s">
         <v>385</v>
       </c>
-      <c r="B191" t="s">
-        <v>6</v>
-      </c>
-      <c r="E191" t="s">
-        <v>386</v>
-      </c>
       <c r="F191" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
+        <v>386</v>
+      </c>
+      <c r="B192" t="s">
+        <v>6</v>
+      </c>
+      <c r="E192" t="s">
         <v>387</v>
       </c>
-      <c r="B192" t="s">
-        <v>6</v>
-      </c>
-      <c r="E192" t="s">
-        <v>388</v>
-      </c>
       <c r="F192" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
+        <v>388</v>
+      </c>
+      <c r="B193" t="s">
+        <v>6</v>
+      </c>
+      <c r="E193" t="s">
         <v>389</v>
       </c>
-      <c r="B193" t="s">
-        <v>6</v>
-      </c>
-      <c r="E193" t="s">
-        <v>390</v>
-      </c>
       <c r="F193" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B194" t="s">
         <v>9</v>
@@ -4828,15 +4829,15 @@
         <v>0</v>
       </c>
       <c r="E194" t="s">
+        <v>391</v>
+      </c>
+      <c r="F194" t="s">
         <v>392</v>
-      </c>
-      <c r="F194" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B195" t="s">
         <v>9</v>
@@ -4848,15 +4849,15 @@
         <v>0</v>
       </c>
       <c r="E195" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F195" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B196" t="s">
         <v>9</v>
@@ -4868,15 +4869,15 @@
         <v>0</v>
       </c>
       <c r="E196" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F196" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B197" t="s">
         <v>8</v>
@@ -4888,220 +4889,220 @@
         <v>1</v>
       </c>
       <c r="E197" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F197" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B198" t="s">
         <v>6</v>
       </c>
       <c r="E198" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F198" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B199" t="s">
         <v>6</v>
       </c>
       <c r="E199" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F199" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B200" t="s">
         <v>6</v>
       </c>
       <c r="E200" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F200" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
+        <v>402</v>
+      </c>
+      <c r="B201" t="s">
+        <v>6</v>
+      </c>
+      <c r="E201" t="s">
         <v>403</v>
       </c>
-      <c r="B201" t="s">
-        <v>6</v>
-      </c>
-      <c r="E201" t="s">
-        <v>404</v>
-      </c>
       <c r="F201" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B202" t="s">
         <v>10</v>
       </c>
       <c r="E202" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F202" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" t="s">
+        <v>6</v>
+      </c>
+      <c r="E203" t="s">
         <v>405</v>
       </c>
-      <c r="B203" t="s">
-        <v>6</v>
-      </c>
-      <c r="E203" t="s">
-        <v>406</v>
-      </c>
       <c r="F203" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" t="s">
+        <v>6</v>
+      </c>
+      <c r="E204" t="s">
         <v>407</v>
       </c>
-      <c r="B204" t="s">
-        <v>6</v>
-      </c>
-      <c r="E204" t="s">
-        <v>408</v>
-      </c>
       <c r="F204" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" t="s">
+        <v>6</v>
+      </c>
+      <c r="E205" t="s">
         <v>409</v>
       </c>
-      <c r="B205" t="s">
-        <v>6</v>
-      </c>
-      <c r="E205" t="s">
-        <v>410</v>
-      </c>
       <c r="F205" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" t="s">
+        <v>6</v>
+      </c>
+      <c r="E206" t="s">
         <v>411</v>
       </c>
-      <c r="B206" t="s">
-        <v>6</v>
-      </c>
-      <c r="E206" t="s">
-        <v>412</v>
-      </c>
       <c r="F206" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" t="s">
+        <v>6</v>
+      </c>
+      <c r="E207" t="s">
         <v>413</v>
       </c>
-      <c r="B207" t="s">
-        <v>6</v>
-      </c>
-      <c r="E207" t="s">
-        <v>414</v>
-      </c>
       <c r="F207" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" t="s">
+        <v>6</v>
+      </c>
+      <c r="E208" t="s">
         <v>415</v>
       </c>
-      <c r="B208" t="s">
-        <v>6</v>
-      </c>
-      <c r="E208" t="s">
-        <v>416</v>
-      </c>
       <c r="F208" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
+        <v>416</v>
+      </c>
+      <c r="B209" t="s">
+        <v>6</v>
+      </c>
+      <c r="E209" t="s">
         <v>417</v>
       </c>
-      <c r="B209" t="s">
-        <v>6</v>
-      </c>
-      <c r="E209" t="s">
-        <v>418</v>
-      </c>
       <c r="F209" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
+        <v>418</v>
+      </c>
+      <c r="B210" t="s">
+        <v>6</v>
+      </c>
+      <c r="E210" t="s">
         <v>419</v>
       </c>
-      <c r="B210" t="s">
-        <v>6</v>
-      </c>
-      <c r="E210" t="s">
-        <v>420</v>
-      </c>
       <c r="F210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
+        <v>420</v>
+      </c>
+      <c r="B211" t="s">
+        <v>6</v>
+      </c>
+      <c r="E211" t="s">
         <v>421</v>
       </c>
-      <c r="B211" t="s">
-        <v>6</v>
-      </c>
-      <c r="E211" t="s">
-        <v>422</v>
-      </c>
       <c r="F211" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>422</v>
+      </c>
+      <c r="B212" t="s">
+        <v>6</v>
+      </c>
+      <c r="E212" t="s">
         <v>423</v>
       </c>
-      <c r="B212" t="s">
-        <v>6</v>
-      </c>
-      <c r="E212" t="s">
-        <v>424</v>
-      </c>
       <c r="F212" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>